<commit_message>
Update Notes - MarketPlace - Data Dictionary.xlsx
</commit_message>
<xml_diff>
--- a/Database/Notes - MarketPlace - Data Dictionary.xlsx
+++ b/Database/Notes - MarketPlace - Data Dictionary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="175">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -769,6 +769,54 @@
   </si>
   <si>
     <t>primary key</t>
+  </si>
+  <si>
+    <t>seller_id</t>
+  </si>
+  <si>
+    <t>approved_by</t>
+  </si>
+  <si>
+    <t>rejected_date</t>
+  </si>
+  <si>
+    <t>rejected_by</t>
+  </si>
+  <si>
+    <t>name of amin who approved respected note</t>
+  </si>
+  <si>
+    <t>which admin rejected respective book</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>date when book is rejected</t>
+  </si>
+  <si>
+    <t>remark for rejection</t>
+  </si>
+  <si>
+    <t>rejected_notes</t>
+  </si>
+  <si>
+    <t>sold_notes</t>
+  </si>
+  <si>
+    <t>download_date</t>
+  </si>
+  <si>
+    <t>foreign key ,buyers id, which is one of the users table</t>
+  </si>
+  <si>
+    <t>foreign key ,book_id of requested book from notes table</t>
+  </si>
+  <si>
+    <t>date download of respective book</t>
+  </si>
+  <si>
+    <t>foreign key , id of seller from users table</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1188,6 +1236,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1197,6 +1257,15 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1214,21 +1283,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,11 +1578,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G154"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D88" sqref="D88"/>
+      <pane ySplit="3" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1542,14 +1596,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="10.5" customHeight="1">
       <c r="A2" s="29"/>
@@ -1581,15 +1635,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" ht="7.5" customHeight="1" thickBot="1">
-      <c r="A4" s="61"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="55" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -1607,7 +1661,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
-      <c r="A6" s="52"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
@@ -1623,7 +1677,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
-      <c r="A7" s="52"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="19" t="s">
         <v>20</v>
       </c>
@@ -1641,7 +1695,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15">
-      <c r="A8" s="52"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="19" t="s">
         <v>21</v>
       </c>
@@ -1659,7 +1713,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A9" s="52"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="19" t="s">
         <v>22</v>
       </c>
@@ -1677,7 +1731,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15">
-      <c r="A10" s="52"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="19" t="s">
         <v>23</v>
       </c>
@@ -1695,7 +1749,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15">
-      <c r="A11" s="52"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="41" t="s">
         <v>9</v>
       </c>
@@ -1711,7 +1765,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15">
-      <c r="A12" s="52"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="19" t="s">
         <v>16</v>
       </c>
@@ -1727,7 +1781,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="45.75" customHeight="1">
-      <c r="A13" s="52"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="19" t="s">
         <v>15</v>
       </c>
@@ -1743,7 +1797,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15">
-      <c r="A14" s="52"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="19" t="s">
         <v>17</v>
       </c>
@@ -1759,7 +1813,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15">
-      <c r="A15" s="52"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="19" t="s">
         <v>18</v>
       </c>
@@ -1775,7 +1829,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" thickBot="1">
-      <c r="A16" s="53"/>
+      <c r="A16" s="57"/>
       <c r="B16" s="21" t="s">
         <v>10</v>
       </c>
@@ -1791,15 +1845,15 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="55" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="15" t="s">
@@ -1817,7 +1871,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15">
-      <c r="A19" s="52"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="19" t="s">
         <v>35</v>
       </c>
@@ -1835,7 +1889,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15">
-      <c r="A20" s="52"/>
+      <c r="A20" s="56"/>
       <c r="B20" s="19" t="s">
         <v>36</v>
       </c>
@@ -1853,7 +1907,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15">
-      <c r="A21" s="52"/>
+      <c r="A21" s="56"/>
       <c r="B21" s="19" t="s">
         <v>16</v>
       </c>
@@ -1869,7 +1923,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15">
-      <c r="A22" s="52"/>
+      <c r="A22" s="56"/>
       <c r="B22" s="19" t="s">
         <v>15</v>
       </c>
@@ -1885,7 +1939,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15">
-      <c r="A23" s="52"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="19" t="s">
         <v>17</v>
       </c>
@@ -1901,7 +1955,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15">
-      <c r="A24" s="52"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="19" t="s">
         <v>18</v>
       </c>
@@ -1917,7 +1971,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A25" s="53"/>
+      <c r="A25" s="57"/>
       <c r="B25" s="21" t="s">
         <v>10</v>
       </c>
@@ -1932,9 +1986,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="26" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
     <row r="27" spans="1:6" ht="15" customHeight="1">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="55" t="s">
         <v>146</v>
       </c>
       <c r="B27" s="15" t="s">
@@ -1952,7 +2006,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
-      <c r="A28" s="52"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="19" t="s">
         <v>45</v>
       </c>
@@ -1968,7 +2022,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
-      <c r="A29" s="52"/>
+      <c r="A29" s="56"/>
       <c r="B29" s="19" t="s">
         <v>48</v>
       </c>
@@ -1986,7 +2040,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
-      <c r="A30" s="52"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="19" t="s">
         <v>50</v>
       </c>
@@ -2004,7 +2058,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1">
-      <c r="A31" s="52"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="19" t="s">
         <v>53</v>
       </c>
@@ -2022,7 +2076,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1">
-      <c r="A32" s="52"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="19" t="s">
         <v>54</v>
       </c>
@@ -2040,7 +2094,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1">
-      <c r="A33" s="52"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="19" t="s">
         <v>55</v>
       </c>
@@ -2058,7 +2112,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
-      <c r="A34" s="52"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="19" t="s">
         <v>57</v>
       </c>
@@ -2076,7 +2130,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1">
-      <c r="A35" s="52"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="19" t="s">
         <v>58</v>
       </c>
@@ -2094,7 +2148,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
-      <c r="A36" s="52"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="19" t="s">
         <v>59</v>
       </c>
@@ -2112,7 +2166,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
-      <c r="A37" s="52"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="19" t="s">
         <v>60</v>
       </c>
@@ -2130,7 +2184,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
-      <c r="A38" s="52"/>
+      <c r="A38" s="56"/>
       <c r="B38" s="19" t="s">
         <v>65</v>
       </c>
@@ -2148,7 +2202,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1">
-      <c r="A39" s="52"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="19" t="s">
         <v>66</v>
       </c>
@@ -2166,7 +2220,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
-      <c r="A40" s="52"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="19" t="s">
         <v>16</v>
       </c>
@@ -2182,7 +2236,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1">
-      <c r="A41" s="52"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="19" t="s">
         <v>15</v>
       </c>
@@ -2198,7 +2252,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1">
-      <c r="A42" s="52"/>
+      <c r="A42" s="56"/>
       <c r="B42" s="19" t="s">
         <v>17</v>
       </c>
@@ -2214,7 +2268,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1">
-      <c r="A43" s="52"/>
+      <c r="A43" s="56"/>
       <c r="B43" s="19" t="s">
         <v>18</v>
       </c>
@@ -2230,7 +2284,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A44" s="53"/>
+      <c r="A44" s="57"/>
       <c r="B44" s="21" t="s">
         <v>10</v>
       </c>
@@ -2245,9 +2299,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="45" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
     <row r="46" spans="1:6" ht="15" customHeight="1">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="55" t="s">
         <v>147</v>
       </c>
       <c r="B46" s="36" t="s">
@@ -2267,7 +2321,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1">
-      <c r="A47" s="52"/>
+      <c r="A47" s="56"/>
       <c r="B47" s="19" t="s">
         <v>50</v>
       </c>
@@ -2285,7 +2339,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1">
-      <c r="A48" s="52"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="19" t="s">
         <v>53</v>
       </c>
@@ -2303,7 +2357,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1">
-      <c r="A49" s="52"/>
+      <c r="A49" s="56"/>
       <c r="B49" s="19" t="s">
         <v>16</v>
       </c>
@@ -2319,7 +2373,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1">
-      <c r="A50" s="52"/>
+      <c r="A50" s="56"/>
       <c r="B50" s="19" t="s">
         <v>15</v>
       </c>
@@ -2335,7 +2389,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1">
-      <c r="A51" s="52"/>
+      <c r="A51" s="56"/>
       <c r="B51" s="19" t="s">
         <v>17</v>
       </c>
@@ -2351,7 +2405,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1">
-      <c r="A52" s="52"/>
+      <c r="A52" s="56"/>
       <c r="B52" s="19" t="s">
         <v>18</v>
       </c>
@@ -2367,7 +2421,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A53" s="53"/>
+      <c r="A53" s="57"/>
       <c r="B53" s="21" t="s">
         <v>10</v>
       </c>
@@ -2382,9 +2436,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="54" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
     <row r="55" spans="1:6" ht="15" customHeight="1">
-      <c r="A55" s="51" t="s">
+      <c r="A55" s="55" t="s">
         <v>148</v>
       </c>
       <c r="B55" s="31" t="s">
@@ -2402,45 +2456,43 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1">
-      <c r="A56" s="52"/>
+      <c r="A56" s="56"/>
       <c r="B56" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="51"/>
+      <c r="E56" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" customHeight="1">
+      <c r="A57" s="56"/>
+      <c r="B57" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="11">
+      <c r="C57" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="11">
         <v>150</v>
       </c>
-      <c r="E56" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" s="34" t="s">
+      <c r="E57" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1">
-      <c r="A57" s="52"/>
-      <c r="B57" s="33" t="s">
+    <row r="58" spans="1:6" ht="15" customHeight="1">
+      <c r="A58" s="56"/>
+      <c r="B58" s="33" t="s">
         <v>109</v>
-      </c>
-      <c r="C57" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57" s="11">
-        <v>100</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" s="34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="15" customHeight="1">
-      <c r="A58" s="52"/>
-      <c r="B58" s="33" t="s">
-        <v>110</v>
       </c>
       <c r="C58" s="33" t="s">
         <v>12</v>
@@ -2452,85 +2504,85 @@
         <v>19</v>
       </c>
       <c r="F58" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" customHeight="1">
+      <c r="A59" s="56"/>
+      <c r="B59" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="11">
+        <v>100</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1">
-      <c r="A59" s="52"/>
-      <c r="B59" s="33" t="s">
+    <row r="60" spans="1:6" ht="15" customHeight="1">
+      <c r="A60" s="56"/>
+      <c r="B60" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C59" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="11">
+      <c r="C60" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="11">
         <v>10</v>
       </c>
-      <c r="E59" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F59" s="34" t="s">
+      <c r="E60" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1">
-      <c r="A60" s="52"/>
-      <c r="B60" s="33" t="s">
+    <row r="61" spans="1:6" ht="15" customHeight="1">
+      <c r="A61" s="56"/>
+      <c r="B61" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="C60" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" s="11" t="s">
+      <c r="C61" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E60" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" s="34" t="s">
+      <c r="E61" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1">
-      <c r="A61" s="52"/>
-      <c r="B61" s="33" t="s">
+    <row r="62" spans="1:6" ht="15" customHeight="1">
+      <c r="A62" s="56"/>
+      <c r="B62" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="C61" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="11">
+      <c r="C62" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="11">
         <v>50</v>
       </c>
-      <c r="E61" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F61" s="34" t="s">
+      <c r="E62" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1">
-      <c r="A62" s="52"/>
-      <c r="B62" s="33" t="s">
+    <row r="63" spans="1:6" ht="15" customHeight="1">
+      <c r="A63" s="56"/>
+      <c r="B63" s="33" t="s">
         <v>119</v>
-      </c>
-      <c r="C62" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="11">
-        <v>100</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F62" s="34" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1">
-      <c r="A63" s="52"/>
-      <c r="B63" s="33" t="s">
-        <v>121</v>
       </c>
       <c r="C63" s="33" t="s">
         <v>12</v>
@@ -2542,13 +2594,13 @@
         <v>24</v>
       </c>
       <c r="F63" s="34" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1">
-      <c r="A64" s="52"/>
+      <c r="A64" s="56"/>
       <c r="B64" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C64" s="33" t="s">
         <v>12</v>
@@ -2560,13 +2612,13 @@
         <v>24</v>
       </c>
       <c r="F64" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1">
-      <c r="A65" s="52"/>
+      <c r="A65" s="56"/>
       <c r="B65" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C65" s="33" t="s">
         <v>12</v>
@@ -2578,113 +2630,115 @@
         <v>24</v>
       </c>
       <c r="F65" s="34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15" customHeight="1">
+      <c r="A66" s="56"/>
+      <c r="B66" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="11">
+        <v>100</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="34" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15" customHeight="1">
-      <c r="A66" s="52"/>
-      <c r="B66" s="33" t="s">
+    <row r="67" spans="1:6" ht="15" customHeight="1">
+      <c r="A67" s="56"/>
+      <c r="B67" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="C66" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="11">
+      <c r="C67" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="11">
         <v>5</v>
       </c>
-      <c r="E66" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F66" s="34" t="s">
+      <c r="E67" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" s="34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1">
-      <c r="A67" s="52"/>
-      <c r="B67" s="33" t="s">
+    <row r="68" spans="1:6" ht="15" customHeight="1">
+      <c r="A68" s="56"/>
+      <c r="B68" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="C67" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D67" s="11">
+      <c r="C68" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="11">
         <v>10</v>
       </c>
-      <c r="E67" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F67" s="34" t="s">
+      <c r="E68" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" s="34" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1">
-      <c r="A68" s="52"/>
-      <c r="B68" s="33" t="s">
+    <row r="69" spans="1:6" ht="15" customHeight="1">
+      <c r="A69" s="56"/>
+      <c r="B69" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="C68" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="33"/>
-      <c r="E68" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F68" s="34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1">
-      <c r="A69" s="52"/>
-      <c r="B69" s="33" t="s">
-        <v>128</v>
-      </c>
       <c r="C69" s="33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D69" s="33"/>
       <c r="E69" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F69" s="34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1">
+      <c r="A70" s="56"/>
+      <c r="B70" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="33"/>
+      <c r="E70" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F70" s="34" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1">
-      <c r="A70" s="52"/>
-      <c r="B70" s="19" t="s">
+    <row r="71" spans="1:6" ht="15" customHeight="1">
+      <c r="A71" s="56"/>
+      <c r="B71" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="33"/>
+      <c r="E71" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="34" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15" customHeight="1">
+      <c r="A72" s="56"/>
+      <c r="B72" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F70" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1">
-      <c r="A71" s="52"/>
-      <c r="B71" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F71" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1">
-      <c r="A72" s="52"/>
-      <c r="B72" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>14</v>
@@ -2694,13 +2748,13 @@
         <v>24</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15" customHeight="1">
-      <c r="A73" s="52"/>
+      <c r="A73" s="56"/>
       <c r="B73" s="19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>11</v>
@@ -2710,100 +2764,100 @@
         <v>24</v>
       </c>
       <c r="F73" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15" customHeight="1">
+      <c r="A74" s="56"/>
+      <c r="B74" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F74" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="15" customHeight="1">
+      <c r="A75" s="56"/>
+      <c r="B75" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F75" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A74" s="53"/>
-      <c r="B74" s="21" t="s">
+    <row r="76" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A76" s="57"/>
+      <c r="B76" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="22" t="s">
+      <c r="C76" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F74" s="24" t="s">
+      <c r="D76" s="23"/>
+      <c r="E76" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
-    <row r="76" spans="1:6" ht="15" customHeight="1">
-      <c r="A76" s="51" t="s">
+    <row r="77" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="78" spans="1:6" ht="15" customHeight="1">
+      <c r="A78" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="31" t="s">
+      <c r="B78" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="C76" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D76" s="17">
+      <c r="C78" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" s="17">
         <v>1</v>
       </c>
-      <c r="E76" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F76" s="32" t="s">
+      <c r="E78" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78" s="32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15" customHeight="1">
-      <c r="A77" s="52"/>
-      <c r="B77" s="33" t="s">
+    <row r="79" spans="1:6" ht="15" customHeight="1">
+      <c r="A79" s="56"/>
+      <c r="B79" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C77" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" s="11">
+      <c r="C79" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="11">
         <v>10</v>
       </c>
-      <c r="E77" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F77" s="34" t="s">
+      <c r="E79" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F79" s="34" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15" customHeight="1">
-      <c r="A78" s="52"/>
-      <c r="B78" s="19" t="s">
+    <row r="80" spans="1:6" ht="15" customHeight="1">
+      <c r="A80" s="56"/>
+      <c r="B80" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F78" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="15" customHeight="1">
-      <c r="A79" s="52"/>
-      <c r="B79" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F79" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1">
-      <c r="A80" s="52"/>
-      <c r="B80" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>14</v>
@@ -2813,13 +2867,13 @@
         <v>24</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15" customHeight="1">
-      <c r="A81" s="52"/>
+      <c r="A81" s="56"/>
       <c r="B81" s="19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>11</v>
@@ -2829,54 +2883,64 @@
         <v>24</v>
       </c>
       <c r="F81" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="15" customHeight="1">
+      <c r="A82" s="56"/>
+      <c r="B82" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="15" customHeight="1">
+      <c r="A83" s="56"/>
+      <c r="B83" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A82" s="53"/>
-      <c r="B82" s="21" t="s">
+    <row r="84" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A84" s="57"/>
+      <c r="B84" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C82" s="22" t="s">
+      <c r="C84" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D82" s="23"/>
-      <c r="E82" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" s="24" t="s">
+      <c r="D84" s="23"/>
+      <c r="E84" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="50" customFormat="1" ht="12" customHeight="1" thickBot="1"/>
-    <row r="84" spans="1:6" ht="15" customHeight="1">
-      <c r="B84" s="46" t="s">
+    <row r="85" spans="1:6" s="54" customFormat="1" ht="12" customHeight="1" thickBot="1"/>
+    <row r="86" spans="1:6" ht="15" customHeight="1">
+      <c r="B86" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C84" s="47" t="s">
+      <c r="C86" s="47" t="s">
         <v>82</v>
-      </c>
-      <c r="D84" s="26"/>
-      <c r="E84" s="26"/>
-      <c r="F84" s="26"/>
-    </row>
-    <row r="85" spans="1:6" ht="15" customHeight="1">
-      <c r="B85" s="48">
-        <v>1</v>
-      </c>
-      <c r="C85" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D85" s="26"/>
-      <c r="E85" s="26"/>
-      <c r="F85" s="26"/>
-    </row>
-    <row r="86" spans="1:6" ht="15" customHeight="1">
-      <c r="B86" s="48">
-        <v>2</v>
-      </c>
-      <c r="C86" s="34" t="s">
-        <v>85</v>
       </c>
       <c r="D86" s="26"/>
       <c r="E86" s="26"/>
@@ -2884,149 +2948,139 @@
     </row>
     <row r="87" spans="1:6" ht="15" customHeight="1">
       <c r="B87" s="48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C87" s="34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D87" s="26"/>
       <c r="E87" s="26"/>
       <c r="F87" s="26"/>
     </row>
-    <row r="88" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B88" s="49">
-        <v>4</v>
-      </c>
-      <c r="C88" s="35" t="s">
-        <v>87</v>
+    <row r="88" spans="1:6" ht="15" customHeight="1">
+      <c r="B88" s="48">
+        <v>2</v>
+      </c>
+      <c r="C88" s="34" t="s">
+        <v>85</v>
       </c>
       <c r="D88" s="26"/>
       <c r="E88" s="26"/>
       <c r="F88" s="26"/>
     </row>
-    <row r="89" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
-    <row r="90" spans="1:6" s="28" customFormat="1" ht="15" customHeight="1">
-      <c r="A90" s="51" t="s">
+    <row r="89" spans="1:6" ht="15" customHeight="1">
+      <c r="B89" s="48">
+        <v>3</v>
+      </c>
+      <c r="C89" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="26"/>
+    </row>
+    <row r="90" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="B90" s="49">
+        <v>4</v>
+      </c>
+      <c r="C90" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
+      <c r="F90" s="26"/>
+    </row>
+    <row r="91" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="92" spans="1:6" s="28" customFormat="1" ht="15" customHeight="1">
+      <c r="A92" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B92" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="C90" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="63"/>
-      <c r="E90" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" s="64" t="s">
+      <c r="C92" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="52"/>
+      <c r="E92" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" s="53" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15" customHeight="1">
-      <c r="A91" s="52"/>
-      <c r="B91" s="33" t="s">
+    <row r="93" spans="1:6" ht="15" customHeight="1">
+      <c r="A93" s="56"/>
+      <c r="B93" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C91" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" s="34" t="s">
+      <c r="C93" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" s="34" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" customHeight="1">
-      <c r="A92" s="52"/>
-      <c r="B92" s="33" t="s">
+    <row r="94" spans="1:6" ht="15" customHeight="1">
+      <c r="A94" s="56"/>
+      <c r="B94" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C92" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" s="34" t="s">
+      <c r="C94" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" s="34" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15" customHeight="1">
-      <c r="A93" s="52"/>
-      <c r="B93" s="33" t="s">
+    <row r="95" spans="1:6" ht="15" customHeight="1">
+      <c r="A95" s="56"/>
+      <c r="B95" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="C93" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" s="27">
+      <c r="C95" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" s="27">
         <v>1</v>
       </c>
-      <c r="E93" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" s="34" t="s">
+      <c r="E95" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" s="34" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15" customHeight="1">
-      <c r="A94" s="52"/>
-      <c r="B94" s="33" t="s">
+    <row r="96" spans="1:6" ht="15" customHeight="1">
+      <c r="A96" s="56"/>
+      <c r="B96" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="C94" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D94" s="27" t="s">
+      <c r="C96" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E94" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" s="34" t="s">
+      <c r="E96" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" s="34" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15" customHeight="1">
-      <c r="A95" s="52"/>
-      <c r="B95" s="19" t="s">
+    <row r="97" spans="1:6" ht="15" customHeight="1">
+      <c r="A97" s="56"/>
+      <c r="B97" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D95" s="27"/>
-      <c r="E95" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F95" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="15" customHeight="1">
-      <c r="A96" s="52"/>
-      <c r="B96" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F96" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="15" customHeight="1">
-      <c r="A97" s="52"/>
-      <c r="B97" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>14</v>
@@ -3036,13 +3090,13 @@
         <v>24</v>
       </c>
       <c r="F97" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="15" customHeight="1">
-      <c r="A98" s="52"/>
+      <c r="A98" s="56"/>
       <c r="B98" s="19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>11</v>
@@ -3052,128 +3106,128 @@
         <v>24</v>
       </c>
       <c r="F98" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="15" customHeight="1">
+      <c r="A99" s="56"/>
+      <c r="B99" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" s="27"/>
+      <c r="E99" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F99" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15" customHeight="1">
+      <c r="A100" s="56"/>
+      <c r="B100" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F100" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A99" s="53"/>
-      <c r="B99" s="21" t="s">
+    <row r="101" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A101" s="57"/>
+      <c r="B101" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C99" s="22" t="s">
+      <c r="C101" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D99" s="23"/>
-      <c r="E99" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" s="24" t="s">
+      <c r="D101" s="23"/>
+      <c r="E101" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
-    <row r="101" spans="1:6" ht="15" customHeight="1">
-      <c r="A101" s="51" t="s">
+    <row r="102" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="103" spans="1:6" ht="15" customHeight="1">
+      <c r="A103" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="B101" s="15" t="s">
+      <c r="B103" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="C101" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D101" s="44"/>
-      <c r="E101" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" s="32" t="s">
+      <c r="C103" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="44"/>
+      <c r="E103" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F103" s="32" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15" customHeight="1">
-      <c r="A102" s="52"/>
-      <c r="B102" s="33" t="s">
+    <row r="104" spans="1:6" ht="15" customHeight="1">
+      <c r="A104" s="56"/>
+      <c r="B104" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C102" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D102" s="33"/>
-      <c r="E102" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" s="34" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="15" customHeight="1">
-      <c r="A103" s="52"/>
-      <c r="B103" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C103" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D103" s="33"/>
-      <c r="E103" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F103" s="34" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="15" customHeight="1">
-      <c r="A104" s="52"/>
-      <c r="B104" s="33" t="s">
-        <v>138</v>
-      </c>
       <c r="C104" s="33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D104" s="33"/>
       <c r="E104" s="45" t="s">
         <v>19</v>
       </c>
       <c r="F104" s="34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="15" customHeight="1">
+      <c r="A105" s="56"/>
+      <c r="B105" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" s="33"/>
+      <c r="E105" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F105" s="34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="15" customHeight="1">
+      <c r="A106" s="56"/>
+      <c r="B106" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C106" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" s="33"/>
+      <c r="E106" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" s="34" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15" customHeight="1">
-      <c r="A105" s="52"/>
-      <c r="B105" s="19" t="s">
+    <row r="107" spans="1:6" ht="15" customHeight="1">
+      <c r="A107" s="56"/>
+      <c r="B107" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F105" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="15" customHeight="1">
-      <c r="A106" s="52"/>
-      <c r="B106" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C106" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F106" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="15" customHeight="1">
-      <c r="A107" s="52"/>
-      <c r="B107" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>14</v>
@@ -3183,13 +3237,13 @@
         <v>24</v>
       </c>
       <c r="F107" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="15" customHeight="1">
-      <c r="A108" s="52"/>
+      <c r="A108" s="56"/>
       <c r="B108" s="19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>11</v>
@@ -3199,612 +3253,600 @@
         <v>24</v>
       </c>
       <c r="F108" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="15" customHeight="1">
+      <c r="A109" s="56"/>
+      <c r="B109" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F109" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="15" customHeight="1">
+      <c r="A110" s="56"/>
+      <c r="B110" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F110" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A109" s="53"/>
-      <c r="B109" s="21" t="s">
+    <row r="111" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A111" s="57"/>
+      <c r="B111" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C109" s="22" t="s">
+      <c r="C111" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D109" s="23"/>
-      <c r="E109" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F109" s="24" t="s">
+      <c r="D111" s="23"/>
+      <c r="E111" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F111" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
-    <row r="111" spans="1:6" ht="15" customHeight="1">
-      <c r="A111" s="57" t="s">
+    <row r="112" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="113" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A113" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B113" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C113" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" s="31"/>
+      <c r="E113" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F113" s="32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A114" s="56"/>
+      <c r="B114" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="C114" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="33"/>
+      <c r="E114" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F114" s="34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A115" s="56"/>
+      <c r="B115" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C115" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="33"/>
+      <c r="E115" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F115" s="34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A116" s="56"/>
+      <c r="B116" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="C116" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E116" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F116" s="34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A117" s="56"/>
+      <c r="B117" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="51"/>
+      <c r="E117" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F117" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A118" s="56"/>
+      <c r="B118" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118" s="51"/>
+      <c r="E118" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F118" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A119" s="56"/>
+      <c r="B119" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" s="51"/>
+      <c r="E119" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F119" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A120" s="56"/>
+      <c r="B120" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120" s="51"/>
+      <c r="E120" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F120" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A121" s="57"/>
+      <c r="B121" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" s="23"/>
+      <c r="E121" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F121" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="123" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A123" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="B123" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C123" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" s="31"/>
+      <c r="E123" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F123" s="32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A124" s="56"/>
+      <c r="B124" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" s="33"/>
+      <c r="E124" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F124" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A125" s="56"/>
+      <c r="B125" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C125" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D125" s="33"/>
+      <c r="E125" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F125" s="34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A126" s="56"/>
+      <c r="B126" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126" s="51"/>
+      <c r="E126" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F126" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A127" s="56"/>
+      <c r="B127" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D127" s="51"/>
+      <c r="E127" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F127" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A128" s="56"/>
+      <c r="B128" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D128" s="51"/>
+      <c r="E128" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F128" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1">
+      <c r="A129" s="56"/>
+      <c r="B129" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" s="51"/>
+      <c r="E129" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F129" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A130" s="57"/>
+      <c r="B130" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C130" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D130" s="23"/>
+      <c r="E130" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F130" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="132" spans="1:6" ht="15" customHeight="1">
+      <c r="A132" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="B111" s="31" t="s">
+      <c r="B132" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C111" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D111" s="17">
+      <c r="C132" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D132" s="17">
         <v>100</v>
       </c>
-      <c r="E111" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F111" s="32" t="s">
+      <c r="E132" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F132" s="32" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15" customHeight="1">
-      <c r="A112" s="58"/>
-      <c r="B112" s="33" t="s">
+    <row r="133" spans="1:6" ht="15" customHeight="1">
+      <c r="A133" s="65"/>
+      <c r="B133" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C112" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D112" s="11">
+      <c r="C133" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D133" s="11">
         <v>10</v>
       </c>
-      <c r="E112" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F112" s="34" t="s">
+      <c r="E133" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F133" s="34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15" customHeight="1">
-      <c r="A113" s="58"/>
-      <c r="B113" s="19" t="s">
+    <row r="134" spans="1:6" ht="15" customHeight="1">
+      <c r="A134" s="65"/>
+      <c r="B134" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C113" s="5" t="s">
+      <c r="C134" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F113" s="20" t="s">
+      <c r="D134" s="11"/>
+      <c r="E134" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F134" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15" customHeight="1">
-      <c r="A114" s="58"/>
-      <c r="B114" s="19" t="s">
+    <row r="135" spans="1:6" ht="15" customHeight="1">
+      <c r="A135" s="65"/>
+      <c r="B135" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C114" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F114" s="20" t="s">
+      <c r="C135" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D135" s="11"/>
+      <c r="E135" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F135" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15" customHeight="1">
-      <c r="A115" s="58"/>
-      <c r="B115" s="19" t="s">
+    <row r="136" spans="1:6" ht="15" customHeight="1">
+      <c r="A136" s="65"/>
+      <c r="B136" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C115" s="5" t="s">
+      <c r="C136" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F115" s="20" t="s">
+      <c r="D136" s="11"/>
+      <c r="E136" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F136" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15" customHeight="1">
-      <c r="A116" s="58"/>
-      <c r="B116" s="19" t="s">
+    <row r="137" spans="1:6" ht="15" customHeight="1">
+      <c r="A137" s="65"/>
+      <c r="B137" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C116" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D116" s="11"/>
-      <c r="E116" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F116" s="20" t="s">
+      <c r="C137" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D137" s="11"/>
+      <c r="E137" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F137" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="59"/>
-      <c r="B117" s="21" t="s">
+    <row r="138" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A138" s="66"/>
+      <c r="B138" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C117" s="22" t="s">
+      <c r="C138" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D117" s="23"/>
-      <c r="E117" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F117" s="24" t="s">
+      <c r="D138" s="23"/>
+      <c r="E138" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F138" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="118" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
-    <row r="119" spans="1:6" ht="15" customHeight="1">
-      <c r="A119" s="51" t="s">
+    <row r="139" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="140" spans="1:6" ht="15" customHeight="1">
+      <c r="A140" s="55" t="s">
         <v>144</v>
       </c>
-      <c r="B119" s="31" t="s">
+      <c r="B140" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="C119" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D119" s="17">
+      <c r="C140" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D140" s="17">
         <v>100</v>
       </c>
-      <c r="E119" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F119" s="32" t="s">
+      <c r="E140" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F140" s="32" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15" customHeight="1">
-      <c r="A120" s="52"/>
-      <c r="B120" s="33" t="s">
+    <row r="141" spans="1:6" ht="15" customHeight="1">
+      <c r="A141" s="56"/>
+      <c r="B141" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C120" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D120" s="11" t="s">
+      <c r="C141" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D141" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E120" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F120" s="34" t="s">
+      <c r="E141" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F141" s="34" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15" customHeight="1">
-      <c r="A121" s="52"/>
-      <c r="B121" s="19" t="s">
+    <row r="142" spans="1:6" ht="15" customHeight="1">
+      <c r="A142" s="56"/>
+      <c r="B142" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C121" s="5" t="s">
+      <c r="C142" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F121" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="15" customHeight="1">
-      <c r="A122" s="52"/>
-      <c r="B122" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C122" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F122" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="15" customHeight="1">
-      <c r="A123" s="52"/>
-      <c r="B123" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F123" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" ht="15" customHeight="1">
-      <c r="A124" s="52"/>
-      <c r="B124" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C124" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F124" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A125" s="53"/>
-      <c r="B125" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C125" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D125" s="23"/>
-      <c r="E125" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F125" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
-    <row r="127" spans="1:6" ht="15" customHeight="1">
-      <c r="A127" s="51" t="s">
-        <v>130</v>
-      </c>
-      <c r="B127" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="C127" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D127" s="17">
-        <v>100</v>
-      </c>
-      <c r="E127" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F127" s="32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="15" customHeight="1">
-      <c r="A128" s="52"/>
-      <c r="B128" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="C128" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D128" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E128" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F128" s="34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="15" customHeight="1">
-      <c r="A129" s="52"/>
-      <c r="B129" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C129" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D129" s="11"/>
-      <c r="E129" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F129" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="15" customHeight="1">
-      <c r="A130" s="52"/>
-      <c r="B130" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D130" s="11"/>
-      <c r="E130" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F130" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="15" customHeight="1">
-      <c r="A131" s="52"/>
-      <c r="B131" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C131" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F131" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1">
-      <c r="A132" s="52"/>
-      <c r="B132" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C132" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F132" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A133" s="53"/>
-      <c r="B133" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C133" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D133" s="23"/>
-      <c r="E133" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F133" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
-    <row r="135" spans="1:6" ht="15" customHeight="1">
-      <c r="A135" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="B135" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C135" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D135" s="17">
-        <v>100</v>
-      </c>
-      <c r="E135" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F135" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="15" customHeight="1">
-      <c r="A136" s="55"/>
-      <c r="B136" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="C136" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D136" s="11">
-        <v>15</v>
-      </c>
-      <c r="E136" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F136" s="34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="15" customHeight="1">
-      <c r="A137" s="55"/>
-      <c r="B137" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C137" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D137" s="11">
-        <v>50</v>
-      </c>
-      <c r="E137" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F137" s="34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" ht="15" customHeight="1">
-      <c r="A138" s="55"/>
-      <c r="B138" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C138" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D138" s="11">
-        <v>300</v>
-      </c>
-      <c r="E138" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F138" s="34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="15" customHeight="1">
-      <c r="A139" s="55"/>
-      <c r="B139" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="C139" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D139" s="11">
-        <v>300</v>
-      </c>
-      <c r="E139" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F139" s="34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="15" customHeight="1">
-      <c r="A140" s="55"/>
-      <c r="B140" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C140" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D140" s="11">
-        <v>300</v>
-      </c>
-      <c r="E140" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F140" s="34" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" ht="15" customHeight="1">
-      <c r="A141" s="55"/>
-      <c r="B141" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C141" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D141" s="11"/>
-      <c r="E141" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F141" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="15" customHeight="1">
-      <c r="A142" s="55"/>
-      <c r="B142" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C142" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F142" s="20" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="15" customHeight="1">
-      <c r="A143" s="55"/>
+      <c r="A143" s="56"/>
       <c r="B143" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D143" s="11"/>
       <c r="E143" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F143" s="20" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="15" customHeight="1">
-      <c r="A144" s="55"/>
+      <c r="A144" s="56"/>
       <c r="B144" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D144" s="11"/>
       <c r="E144" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F144" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="15" customHeight="1">
+      <c r="A145" s="56"/>
+      <c r="B145" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D145" s="11"/>
+      <c r="E145" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F145" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A145" s="56"/>
-      <c r="B145" s="21" t="s">
+    <row r="146" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A146" s="57"/>
+      <c r="B146" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C145" s="22" t="s">
+      <c r="C146" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D145" s="23"/>
-      <c r="E145" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F145" s="24" t="s">
+      <c r="D146" s="23"/>
+      <c r="E146" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F146" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="146" spans="1:6" s="50" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
-    <row r="147" spans="1:6" ht="15" customHeight="1">
-      <c r="A147" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="B147" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C147" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D147" s="17"/>
-      <c r="E147" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F147" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="147" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
     <row r="148" spans="1:6" ht="15" customHeight="1">
-      <c r="A148" s="52"/>
-      <c r="B148" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C148" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F148" s="34" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="15">
-      <c r="A149" s="52"/>
+      <c r="A148" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B148" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C148" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D148" s="17">
+        <v>100</v>
+      </c>
+      <c r="E148" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F148" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="15" customHeight="1">
+      <c r="A149" s="56"/>
       <c r="B149" s="33" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="C149" s="33" t="s">
         <v>12</v>
@@ -3816,11 +3858,11 @@
         <v>19</v>
       </c>
       <c r="F149" s="34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="15">
-      <c r="A150" s="52"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="15" customHeight="1">
+      <c r="A150" s="56"/>
       <c r="B150" s="19" t="s">
         <v>16</v>
       </c>
@@ -3835,8 +3877,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15">
-      <c r="A151" s="52"/>
+    <row r="151" spans="1:6" ht="15" customHeight="1">
+      <c r="A151" s="56"/>
       <c r="B151" s="19" t="s">
         <v>15</v>
       </c>
@@ -3851,8 +3893,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15">
-      <c r="A152" s="52"/>
+    <row r="152" spans="1:6" ht="15" customHeight="1">
+      <c r="A152" s="56"/>
       <c r="B152" s="19" t="s">
         <v>17</v>
       </c>
@@ -3867,8 +3909,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15">
-      <c r="A153" s="52"/>
+    <row r="153" spans="1:6" ht="15" customHeight="1">
+      <c r="A153" s="56"/>
       <c r="B153" s="19" t="s">
         <v>18</v>
       </c>
@@ -3883,8 +3925,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A154" s="53"/>
+    <row r="154" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A154" s="57"/>
       <c r="B154" s="21" t="s">
         <v>10</v>
       </c>
@@ -3899,10 +3941,350 @@
         <v>34</v>
       </c>
     </row>
+    <row r="155" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="156" spans="1:6" ht="15" customHeight="1">
+      <c r="A156" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="B156" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C156" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D156" s="17">
+        <v>100</v>
+      </c>
+      <c r="E156" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F156" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="15" customHeight="1">
+      <c r="A157" s="62"/>
+      <c r="B157" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C157" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D157" s="11">
+        <v>15</v>
+      </c>
+      <c r="E157" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F157" s="34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="15" customHeight="1">
+      <c r="A158" s="62"/>
+      <c r="B158" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C158" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D158" s="11">
+        <v>50</v>
+      </c>
+      <c r="E158" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F158" s="34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="15" customHeight="1">
+      <c r="A159" s="62"/>
+      <c r="B159" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C159" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D159" s="11">
+        <v>300</v>
+      </c>
+      <c r="E159" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F159" s="34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="15" customHeight="1">
+      <c r="A160" s="62"/>
+      <c r="B160" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C160" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D160" s="11">
+        <v>300</v>
+      </c>
+      <c r="E160" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F160" s="34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="15" customHeight="1">
+      <c r="A161" s="62"/>
+      <c r="B161" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C161" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D161" s="11">
+        <v>300</v>
+      </c>
+      <c r="E161" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F161" s="34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="15" customHeight="1">
+      <c r="A162" s="62"/>
+      <c r="B162" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162" s="11"/>
+      <c r="E162" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F162" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="15" customHeight="1">
+      <c r="A163" s="62"/>
+      <c r="B163" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D163" s="11"/>
+      <c r="E163" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F163" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="15" customHeight="1">
+      <c r="A164" s="62"/>
+      <c r="B164" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D164" s="11"/>
+      <c r="E164" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F164" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="15" customHeight="1">
+      <c r="A165" s="62"/>
+      <c r="B165" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D165" s="11"/>
+      <c r="E165" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F165" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A166" s="63"/>
+      <c r="B166" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C166" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D166" s="23"/>
+      <c r="E166" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F166" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" s="54" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
+    <row r="168" spans="1:6" ht="15" customHeight="1">
+      <c r="A168" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="B168" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C168" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168" s="17"/>
+      <c r="E168" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F168" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="15" customHeight="1">
+      <c r="A169" s="56"/>
+      <c r="B169" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C169" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D169" s="11"/>
+      <c r="E169" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F169" s="34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="15">
+      <c r="A170" s="56"/>
+      <c r="B170" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C170" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D170" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E170" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F170" s="34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="15">
+      <c r="A171" s="56"/>
+      <c r="B171" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D171" s="11"/>
+      <c r="E171" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F171" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="15">
+      <c r="A172" s="56"/>
+      <c r="B172" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D172" s="11"/>
+      <c r="E172" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F172" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="15">
+      <c r="A173" s="56"/>
+      <c r="B173" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D173" s="11"/>
+      <c r="E173" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F173" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="15">
+      <c r="A174" s="56"/>
+      <c r="B174" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D174" s="11"/>
+      <c r="E174" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F174" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A175" s="57"/>
+      <c r="B175" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C175" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D175" s="23"/>
+      <c r="E175" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F175" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="A118:XFD118"/>
-    <mergeCell ref="A90:A99"/>
+  <mergeCells count="32">
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="A103:A111"/>
+    <mergeCell ref="A132:A138"/>
+    <mergeCell ref="A91:XFD91"/>
+    <mergeCell ref="A85:XFD85"/>
+    <mergeCell ref="A122:XFD122"/>
+    <mergeCell ref="A113:A121"/>
+    <mergeCell ref="A123:A130"/>
+    <mergeCell ref="A131:XFD131"/>
+    <mergeCell ref="A168:A175"/>
+    <mergeCell ref="A167:XFD167"/>
+    <mergeCell ref="A140:A146"/>
+    <mergeCell ref="A148:A154"/>
+    <mergeCell ref="A156:A166"/>
+    <mergeCell ref="A155:XFD155"/>
+    <mergeCell ref="A147:XFD147"/>
+    <mergeCell ref="A139:XFD139"/>
+    <mergeCell ref="A92:A101"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A18:A25"/>
@@ -3910,25 +4292,13 @@
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A27:A44"/>
     <mergeCell ref="A45:XFD45"/>
-    <mergeCell ref="A55:A74"/>
+    <mergeCell ref="A55:A76"/>
     <mergeCell ref="A26:XFD26"/>
     <mergeCell ref="A46:A53"/>
     <mergeCell ref="A54:XFD54"/>
-    <mergeCell ref="A75:XFD75"/>
-    <mergeCell ref="A147:A154"/>
-    <mergeCell ref="A146:XFD146"/>
-    <mergeCell ref="A119:A125"/>
-    <mergeCell ref="A127:A133"/>
-    <mergeCell ref="A135:A145"/>
-    <mergeCell ref="A110:XFD110"/>
-    <mergeCell ref="A100:XFD100"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="A101:A109"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A89:XFD89"/>
-    <mergeCell ref="A83:XFD83"/>
-    <mergeCell ref="A134:XFD134"/>
-    <mergeCell ref="A126:XFD126"/>
+    <mergeCell ref="A77:XFD77"/>
+    <mergeCell ref="A112:XFD112"/>
+    <mergeCell ref="A102:XFD102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3949,12 +4319,151 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C9:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="9" spans="3:7" ht="15.75" thickBot="1"/>
+    <row r="10" spans="3:7">
+      <c r="C10" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7">
+      <c r="C11" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="33"/>
+      <c r="F11" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7">
+      <c r="C12" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7">
+      <c r="C13" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7">
+      <c r="C14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7">
+      <c r="C16" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="15.75" thickBot="1">
+      <c r="C18" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>